<commit_message>
Update QIA scraper with granular geographic taxonomy
Implemented refined geographic categorization system per requirements:
- UK (7 deals)
- Europe (excluding UK) - 9 deals
- United States (8 deals)
- Asia - Developed: Japan, South Korea, Singapore, Hong Kong (2 deals)
- Asia - Emerging: China, India, Southeast Asia excl. Singapore (8 deals)
- Middle East & North Africa (1 deal)
- Sub-Saharan Africa (2 deals)
- Latin America (1 deal)
- Australia/Oceania (1 deal)
- Global/Multi-region (2 deals)

Changes:
- Updated all 42 deals with new geographic classifications
- Regenerated CSV/Excel output files with updated taxonomy
- Enhanced README with geographic taxonomy documentation
- Added detailed category definitions

All deals remain the same (42 total), only geographic categorization
has been refined for more granular regional analysis.

Version: 2.0 (Updated Geographic Taxonomy)
</commit_message>
<xml_diff>
--- a/scrapers/qia_investment_deals.xlsx
+++ b/scrapers/qia_investment_deals.xlsx
@@ -436,7 +436,7 @@
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="45" customWidth="1" min="3" max="3"/>
-    <col width="31" customWidth="1" min="4" max="4"/>
+    <col width="28" customWidth="1" min="4" max="4"/>
     <col width="41" customWidth="1" min="5" max="5"/>
     <col width="50" customWidth="1" min="6" max="6"/>
     <col width="32" customWidth="1" min="7" max="7"/>
@@ -501,7 +501,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Qatar/Global</t>
+          <t>Global/Multi-region</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>Asia - Emerging</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Latin America</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Canada (operations in Africa)</t>
+          <t>Sub-Saharan Africa</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>United States/Global</t>
+          <t>Global/Multi-region</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Asia - Emerging</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Asia - Emerging</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Asia - Developed</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>China/Hong Kong</t>
+          <t>Asia - Emerging</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Germany/Europe</t>
+          <t>Europe (excluding UK)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Switzerland/Europe</t>
+          <t>Europe (excluding UK)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Asia - Emerging</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Australia/Oceania</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>France/Europe</t>
+          <t>Europe (excluding UK)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Asia - Emerging</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Asia - Emerging</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Turkey/Emerging Markets</t>
+          <t>Middle East &amp; North Africa</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Germany/Europe</t>
+          <t>Europe (excluding UK)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Africa/Emerging Markets</t>
+          <t>Sub-Saharan Africa</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>India/Asia</t>
+          <t>Asia - Emerging</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Hong Kong/Asia</t>
+          <t>Asia - Developed</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>France/Europe</t>
+          <t>Europe (excluding UK)</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>United Kingdom/Europe</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>United Kingdom/Europe</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>United Kingdom/Europe</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>United Kingdom/Europe</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>United Kingdom/Europe</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Germany/Europe</t>
+          <t>Europe (excluding UK)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Spain/Europe</t>
+          <t>Europe (excluding UK)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Germany/Europe</t>
+          <t>Europe (excluding UK)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>United Kingdom/Europe</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Germany/Europe</t>
+          <t>Europe (excluding UK)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">

</xml_diff>